<commit_message>
Update project. Separata all tables in different files.
</commit_message>
<xml_diff>
--- a/Tables/IpTable.xlsx
+++ b/Tables/IpTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mRaVk\Desktop\CNProject11D21N\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mRaVk\Desktop\Computer-networks-certificate-work-ipIssue\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="90">
   <si>
     <t>Device</t>
   </si>
@@ -282,30 +282,6 @@
   </si>
   <si>
     <t>WI</t>
-  </si>
-  <si>
-    <t>Network</t>
-  </si>
-  <si>
-    <t>Next Hop</t>
-  </si>
-  <si>
-    <t>192.16.1.2</t>
-  </si>
-  <si>
-    <t>192.16.1.4</t>
-  </si>
-  <si>
-    <t>192.16.1.5</t>
-  </si>
-  <si>
-    <t>192.16.1.6</t>
-  </si>
-  <si>
-    <t>192.16.1.7</t>
-  </si>
-  <si>
-    <t>192.16.1.3</t>
   </si>
   <si>
     <t>Printer1</t>
@@ -369,15 +345,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -662,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1389,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>55</v>
@@ -1425,7 +1398,7 @@
         <v>16</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>13</v>
@@ -1436,7 +1409,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>55</v>
@@ -1445,7 +1418,7 @@
         <v>16</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>13</v>
@@ -1454,817 +1427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F47" s="5"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F54" s="5"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F55" s="5"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" s="5"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F57" s="5"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" s="5"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F61" s="5"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F62" s="5"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F63" s="5"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F64" s="5"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F65" s="5"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F66" s="5"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F69" s="5"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F70" s="5"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F71" s="5"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F72" s="5"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F73" s="5"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F74" s="5"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F78" s="5"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F79" s="5"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F80" s="5"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F81" s="5"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F82" s="5"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F85" s="5"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F86" s="5"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F87" s="5"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F88" s="5"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F89" s="5"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F90" s="5"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F93" s="5"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F94" s="5"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F95" s="5"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F96" s="5"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F97" s="5"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F98" s="5"/>
-    </row>
   </sheetData>
-  <mergeCells count="136">
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="A60:F60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="E82:F82"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="A84:F84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="A92:F92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="E93:F93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="E96:F96"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>